<commit_message>
Creating a new saf case study
</commit_message>
<xml_diff>
--- a/src/technology/pv-residential-simple/pv-residential-simple.xlsx
+++ b/src/technology/pv-residential-simple/pv-residential-simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\pv-residential-simple\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/src/technology/pv-residential-simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DDC74F-D1DF-43CB-9640-73847D25382F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{10DDC74F-D1DF-43CB-9640-73847D25382F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324C0ACE-23DA-3A4C-B19A-174C517FB3B4}"/>
   <bookViews>
-    <workbookView xWindow="11010" yWindow="3270" windowWidth="16020" windowHeight="11715" activeTab="5" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
+    <workbookView xWindow="11020" yWindow="3280" windowWidth="16020" windowHeight="11720" activeTab="3" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
   </bookViews>
   <sheets>
     <sheet name="indices" sheetId="1" r:id="rId1"/>
@@ -688,6 +688,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,9 +995,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1013,7 +1017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1030,7 +1034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1081,7 +1085,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1098,7 +1102,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1115,7 +1119,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1132,7 +1136,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1160,9 +1164,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1188,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1220,13 +1224,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB20890-62B7-47AF-BA68-650F053D99C5}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1249,7 +1257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1272,7 +1280,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1295,7 +1303,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1338,7 +1346,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1361,7 +1369,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1384,7 +1392,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1407,7 +1415,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1430,7 +1438,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1484,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1530,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1542,7 +1550,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1565,7 +1573,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1588,7 +1596,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1611,7 +1619,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1634,7 +1642,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1657,7 +1665,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1680,7 +1688,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1703,7 +1711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1726,7 +1734,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1746,7 +1754,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1769,7 +1777,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1792,7 +1800,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1815,7 +1823,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1838,7 +1846,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1861,7 +1869,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1884,7 +1892,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1907,7 +1915,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1930,7 +1938,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1950,7 +1958,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1973,7 +1981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1996,7 +2004,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2019,7 +2027,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -2042,7 +2050,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -2065,7 +2073,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -2088,7 +2096,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -2111,7 +2119,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -2134,7 +2142,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -2154,7 +2162,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -2177,7 +2185,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -2200,7 +2208,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -2223,7 +2231,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -2246,7 +2254,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -2269,7 +2277,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -2292,7 +2300,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -2315,7 +2323,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -2338,7 +2346,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2358,7 +2366,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2381,7 +2389,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -2404,7 +2412,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -2427,7 +2435,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -2450,7 +2458,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -2473,7 +2481,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -2496,7 +2504,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -2519,7 +2527,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -2542,7 +2550,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -2562,7 +2570,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -2585,7 +2593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -2608,7 +2616,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -2631,7 +2639,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -2654,7 +2662,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>31</v>
       </c>
@@ -2677,7 +2685,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>31</v>
       </c>
@@ -2700,7 +2708,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -2723,7 +2731,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>31</v>
       </c>
@@ -2746,7 +2754,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -2766,7 +2774,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>31</v>
       </c>
@@ -2789,7 +2797,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -2812,7 +2820,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>31</v>
       </c>
@@ -2835,7 +2843,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -2858,7 +2866,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -2881,7 +2889,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>31</v>
       </c>
@@ -2904,7 +2912,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -2927,7 +2935,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>31</v>
       </c>
@@ -2950,7 +2958,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>31</v>
       </c>
@@ -2970,7 +2978,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>31</v>
       </c>
@@ -2993,7 +3001,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>31</v>
       </c>
@@ -3016,7 +3024,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>31</v>
       </c>
@@ -3039,7 +3047,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>31</v>
       </c>
@@ -3062,7 +3070,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>31</v>
       </c>
@@ -3085,7 +3093,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -3108,7 +3116,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -3131,7 +3139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>31</v>
       </c>
@@ -3154,7 +3162,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -3174,7 +3182,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>31</v>
       </c>
@@ -3197,7 +3205,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>31</v>
       </c>
@@ -3220,7 +3228,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>31</v>
       </c>
@@ -3243,7 +3251,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>31</v>
       </c>
@@ -3266,7 +3274,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>31</v>
       </c>
@@ -3298,11 +3306,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9375A35C-8A58-4D70-9436-2E641DE51D25}">
   <dimension ref="A1:G211"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -3325,7 +3340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3348,7 +3363,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3371,7 +3386,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -3394,7 +3409,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -3417,7 +3432,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3440,7 +3455,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -3463,7 +3478,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -3509,7 +3524,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -3532,7 +3547,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3555,7 +3570,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3578,7 +3593,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3601,7 +3616,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -3624,7 +3639,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -3647,7 +3662,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -3670,7 +3685,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -3693,7 +3708,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -3716,7 +3731,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -3739,7 +3754,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -3762,7 +3777,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -3785,7 +3800,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -3808,7 +3823,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3831,7 +3846,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -3854,7 +3869,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3877,7 +3892,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -3900,7 +3915,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3923,7 +3938,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -3946,7 +3961,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -3969,7 +3984,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3992,7 +4007,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -4015,7 +4030,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -4038,7 +4053,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -4061,7 +4076,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -4084,7 +4099,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -4107,7 +4122,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -4130,7 +4145,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -4153,7 +4168,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -4176,7 +4191,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -4199,7 +4214,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -4222,7 +4237,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -4245,7 +4260,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -4268,7 +4283,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -4291,7 +4306,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -4314,7 +4329,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -4337,7 +4352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -4360,7 +4375,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -4383,7 +4398,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -4406,7 +4421,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -4429,7 +4444,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -4452,7 +4467,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -4475,7 +4490,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -4498,7 +4513,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -4521,7 +4536,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -4544,7 +4559,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -4567,7 +4582,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -4590,7 +4605,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -4613,7 +4628,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -4636,7 +4651,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -4659,7 +4674,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -4682,7 +4697,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -4705,7 +4720,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -4728,7 +4743,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>31</v>
       </c>
@@ -4751,7 +4766,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>31</v>
       </c>
@@ -4774,7 +4789,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>31</v>
       </c>
@@ -4797,7 +4812,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -4820,7 +4835,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>31</v>
       </c>
@@ -4843,7 +4858,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -4866,7 +4881,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>31</v>
       </c>
@@ -4889,7 +4904,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -4912,7 +4927,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>31</v>
       </c>
@@ -4935,7 +4950,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -4958,7 +4973,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>31</v>
       </c>
@@ -4981,7 +4996,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>31</v>
       </c>
@@ -5004,7 +5019,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>31</v>
       </c>
@@ -5027,7 +5042,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>31</v>
       </c>
@@ -5050,7 +5065,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>31</v>
       </c>
@@ -5073,7 +5088,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>31</v>
       </c>
@@ -5096,7 +5111,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>31</v>
       </c>
@@ -5119,7 +5134,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>31</v>
       </c>
@@ -5142,7 +5157,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>31</v>
       </c>
@@ -5165,7 +5180,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>31</v>
       </c>
@@ -5188,7 +5203,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>31</v>
       </c>
@@ -5211,7 +5226,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>31</v>
       </c>
@@ -5234,7 +5249,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>31</v>
       </c>
@@ -5257,7 +5272,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -5280,7 +5295,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>31</v>
       </c>
@@ -5303,7 +5318,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>31</v>
       </c>
@@ -5326,7 +5341,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>31</v>
       </c>
@@ -5349,7 +5364,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>31</v>
       </c>
@@ -5372,7 +5387,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>31</v>
       </c>
@@ -5395,7 +5410,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>31</v>
       </c>
@@ -5418,7 +5433,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>31</v>
       </c>
@@ -5441,7 +5456,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>31</v>
       </c>
@@ -5464,7 +5479,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>31</v>
       </c>
@@ -5487,7 +5502,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>31</v>
       </c>
@@ -5510,7 +5525,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>31</v>
       </c>
@@ -5533,7 +5548,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>31</v>
       </c>
@@ -5556,7 +5571,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>31</v>
       </c>
@@ -5579,7 +5594,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>31</v>
       </c>
@@ -5602,7 +5617,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>31</v>
       </c>
@@ -5625,7 +5640,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>31</v>
       </c>
@@ -5648,7 +5663,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>31</v>
       </c>
@@ -5671,7 +5686,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>31</v>
       </c>
@@ -5694,7 +5709,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>31</v>
       </c>
@@ -5717,7 +5732,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>31</v>
       </c>
@@ -5740,7 +5755,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>31</v>
       </c>
@@ -5763,7 +5778,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>31</v>
       </c>
@@ -5786,7 +5801,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>31</v>
       </c>
@@ -5809,7 +5824,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>31</v>
       </c>
@@ -5832,7 +5847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>31</v>
       </c>
@@ -5855,7 +5870,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>31</v>
       </c>
@@ -5878,7 +5893,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>31</v>
       </c>
@@ -5901,7 +5916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>31</v>
       </c>
@@ -5924,7 +5939,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>31</v>
       </c>
@@ -5947,7 +5962,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>31</v>
       </c>
@@ -5970,7 +5985,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>31</v>
       </c>
@@ -5993,7 +6008,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>31</v>
       </c>
@@ -6016,7 +6031,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>31</v>
       </c>
@@ -6039,7 +6054,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>31</v>
       </c>
@@ -6062,7 +6077,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>31</v>
       </c>
@@ -6085,7 +6100,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>31</v>
       </c>
@@ -6108,7 +6123,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>31</v>
       </c>
@@ -6131,7 +6146,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>31</v>
       </c>
@@ -6154,7 +6169,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>31</v>
       </c>
@@ -6177,7 +6192,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>31</v>
       </c>
@@ -6200,7 +6215,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>31</v>
       </c>
@@ -6223,7 +6238,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>31</v>
       </c>
@@ -6246,7 +6261,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>31</v>
       </c>
@@ -6269,7 +6284,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>31</v>
       </c>
@@ -6292,7 +6307,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>31</v>
       </c>
@@ -6315,7 +6330,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>31</v>
       </c>
@@ -6338,7 +6353,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>31</v>
       </c>
@@ -6361,7 +6376,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>31</v>
       </c>
@@ -6384,7 +6399,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>31</v>
       </c>
@@ -6407,7 +6422,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>31</v>
       </c>
@@ -6430,7 +6445,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>31</v>
       </c>
@@ -6453,7 +6468,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>31</v>
       </c>
@@ -6476,7 +6491,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>31</v>
       </c>
@@ -6499,7 +6514,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>31</v>
       </c>
@@ -6522,7 +6537,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>31</v>
       </c>
@@ -6545,7 +6560,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>31</v>
       </c>
@@ -6568,7 +6583,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>31</v>
       </c>
@@ -6591,7 +6606,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>31</v>
       </c>
@@ -6614,7 +6629,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>31</v>
       </c>
@@ -6637,7 +6652,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -6660,7 +6675,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>31</v>
       </c>
@@ -6683,7 +6698,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -6706,7 +6721,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>31</v>
       </c>
@@ -6729,7 +6744,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>31</v>
       </c>
@@ -6752,7 +6767,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>31</v>
       </c>
@@ -6775,7 +6790,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>31</v>
       </c>
@@ -6798,7 +6813,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>31</v>
       </c>
@@ -6821,7 +6836,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>31</v>
       </c>
@@ -6844,7 +6859,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>31</v>
       </c>
@@ -6867,7 +6882,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>31</v>
       </c>
@@ -6890,7 +6905,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>31</v>
       </c>
@@ -6913,7 +6928,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>31</v>
       </c>
@@ -6936,7 +6951,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>31</v>
       </c>
@@ -6959,7 +6974,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>31</v>
       </c>
@@ -6982,7 +6997,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>31</v>
       </c>
@@ -7005,7 +7020,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>31</v>
       </c>
@@ -7028,7 +7043,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>31</v>
       </c>
@@ -7051,7 +7066,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>31</v>
       </c>
@@ -7074,7 +7089,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>31</v>
       </c>
@@ -7097,7 +7112,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>31</v>
       </c>
@@ -7120,7 +7135,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>31</v>
       </c>
@@ -7143,7 +7158,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>31</v>
       </c>
@@ -7166,7 +7181,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>31</v>
       </c>
@@ -7189,7 +7204,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>31</v>
       </c>
@@ -7212,7 +7227,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>31</v>
       </c>
@@ -7235,7 +7250,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>31</v>
       </c>
@@ -7258,7 +7273,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>31</v>
       </c>
@@ -7281,7 +7296,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>31</v>
       </c>
@@ -7304,7 +7319,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>31</v>
       </c>
@@ -7327,7 +7342,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>31</v>
       </c>
@@ -7350,7 +7365,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>31</v>
       </c>
@@ -7373,7 +7388,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>31</v>
       </c>
@@ -7396,7 +7411,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>31</v>
       </c>
@@ -7419,7 +7434,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>31</v>
       </c>
@@ -7442,7 +7457,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>31</v>
       </c>
@@ -7465,7 +7480,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>31</v>
       </c>
@@ -7488,7 +7503,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>31</v>
       </c>
@@ -7511,7 +7526,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>31</v>
       </c>
@@ -7534,7 +7549,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>31</v>
       </c>
@@ -7557,7 +7572,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>31</v>
       </c>
@@ -7580,7 +7595,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>31</v>
       </c>
@@ -7603,7 +7618,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>31</v>
       </c>
@@ -7626,7 +7641,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>31</v>
       </c>
@@ -7649,7 +7664,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>31</v>
       </c>
@@ -7672,7 +7687,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>31</v>
       </c>
@@ -7695,7 +7710,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>31</v>
       </c>
@@ -7718,7 +7733,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>31</v>
       </c>
@@ -7741,7 +7756,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>31</v>
       </c>
@@ -7764,7 +7779,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>31</v>
       </c>
@@ -7787,7 +7802,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>31</v>
       </c>
@@ -7810,7 +7825,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>31</v>
       </c>
@@ -7833,7 +7848,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>31</v>
       </c>
@@ -7856,7 +7871,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>31</v>
       </c>
@@ -7879,7 +7894,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>31</v>
       </c>
@@ -7902,7 +7917,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>31</v>
       </c>
@@ -7925,7 +7940,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>31</v>
       </c>
@@ -7948,7 +7963,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>31</v>
       </c>
@@ -7971,7 +7986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>31</v>
       </c>
@@ -7994,7 +8009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>31</v>
       </c>
@@ -8017,7 +8032,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>31</v>
       </c>
@@ -8040,7 +8055,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>31</v>
       </c>
@@ -8063,7 +8078,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>31</v>
       </c>
@@ -8086,7 +8101,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>31</v>
       </c>
@@ -8109,7 +8124,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>31</v>
       </c>
@@ -8132,7 +8147,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>31</v>
       </c>
@@ -8166,9 +8181,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -8185,7 +8200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -8199,7 +8214,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -8213,7 +8228,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -8230,7 +8245,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -8247,7 +8262,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -8273,11 +8288,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D89E1871-0EA4-4433-AFC4-28BCC91530B9}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8294,7 +8309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -8308,7 +8323,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -8322,7 +8337,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -8336,7 +8351,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -8350,7 +8365,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -8364,7 +8379,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -8378,7 +8393,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -8392,7 +8407,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -8406,7 +8421,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -8433,9 +8448,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>161</v>
       </c>
@@ -8449,7 +8464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -8460,7 +8475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>162</v>
       </c>
@@ -8471,7 +8486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -8482,7 +8497,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -8493,7 +8508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -8504,7 +8519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -8515,7 +8530,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -8526,7 +8541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -8537,7 +8552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>164</v>
       </c>

</xml_diff>